<commit_message>
updated BD SPP goal with improved species list; added a placeholder for pressures descriptions on the web
</commit_message>
<xml_diff>
--- a/prep/SPP/spp_coastal_birds.xlsx
+++ b/prep/SPP/spp_coastal_birds.xlsx
@@ -1,17 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28615"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eschemmel/Documents/github/mhi/prep/SPP/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1275" windowWidth="22995" windowHeight="8895"/>
+    <workbookView xWindow="1440" yWindow="1280" windowWidth="23000" windowHeight="11540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -230,12 +243,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -265,12 +278,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -480,9 +493,13 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -496,7 +513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -504,7 +521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -512,7 +529,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -523,7 +540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -531,7 +548,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -539,7 +556,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -547,7 +564,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -555,7 +572,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -563,7 +580,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -571,7 +588,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -579,7 +596,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -590,7 +607,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -598,7 +615,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -606,7 +623,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -614,7 +631,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -622,7 +639,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -630,7 +647,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -649,7 +666,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -661,7 +678,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>